<commit_message>
Added Firebase, getting questions from cloud, started user login
</commit_message>
<xml_diff>
--- a/fakeUserNames.xlsx
+++ b/fakeUserNames.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\musta\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Belgeler\triviachallanger\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="153">
   <si>
     <t>AliKral</t>
   </si>
@@ -442,6 +442,42 @@
   </si>
   <si>
     <t>false</t>
+  </si>
+  <si>
+    <t>çılgın çiçek</t>
+  </si>
+  <si>
+    <t>cici patates</t>
+  </si>
+  <si>
+    <t>Quickduck</t>
+  </si>
+  <si>
+    <t>FakırKral</t>
+  </si>
+  <si>
+    <t>UçanTekmeCetLi</t>
+  </si>
+  <si>
+    <t>RunAway</t>
+  </si>
+  <si>
+    <t>HomePhobiA</t>
+  </si>
+  <si>
+    <t>cehape</t>
+  </si>
+  <si>
+    <t>MarlonBrando</t>
+  </si>
+  <si>
+    <t>NaylonBranda</t>
+  </si>
+  <si>
+    <t>SweetHomeBursa</t>
+  </si>
+  <si>
+    <t>Tarhanatula</t>
   </si>
 </sst>
 </file>
@@ -1266,13 +1302,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C139"/>
+  <dimension ref="A1:C151"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="A152" sqref="A152"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -2802,6 +2840,138 @@
       </c>
       <c r="C139">
         <v>33000</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>141</v>
+      </c>
+      <c r="B140" t="s">
+        <v>140</v>
+      </c>
+      <c r="C140">
+        <v>5200</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>142</v>
+      </c>
+      <c r="B141" t="s">
+        <v>140</v>
+      </c>
+      <c r="C141">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>143</v>
+      </c>
+      <c r="B142" t="s">
+        <v>137</v>
+      </c>
+      <c r="C142">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>151</v>
+      </c>
+      <c r="B143" t="s">
+        <v>140</v>
+      </c>
+      <c r="C143">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>146</v>
+      </c>
+      <c r="B144" t="s">
+        <v>140</v>
+      </c>
+      <c r="C144">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>147</v>
+      </c>
+      <c r="B145" t="s">
+        <v>140</v>
+      </c>
+      <c r="C145">
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>144</v>
+      </c>
+      <c r="B146" t="s">
+        <v>137</v>
+      </c>
+      <c r="C146">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>145</v>
+      </c>
+      <c r="B147" t="s">
+        <v>137</v>
+      </c>
+      <c r="C147">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>148</v>
+      </c>
+      <c r="B148" t="s">
+        <v>137</v>
+      </c>
+      <c r="C148">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>149</v>
+      </c>
+      <c r="B149" t="s">
+        <v>137</v>
+      </c>
+      <c r="C149">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>150</v>
+      </c>
+      <c r="B150" t="s">
+        <v>137</v>
+      </c>
+      <c r="C150">
+        <v>22000</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>152</v>
+      </c>
+      <c r="B151" t="s">
+        <v>140</v>
+      </c>
+      <c r="C151">
+        <v>58000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Game almost ready for beta testing
</commit_message>
<xml_diff>
--- a/fakeUserNames.xlsx
+++ b/fakeUserNames.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Belgeler\triviachallanger\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\musta\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="141">
   <si>
     <t>AliKral</t>
   </si>
@@ -442,42 +442,6 @@
   </si>
   <si>
     <t>false</t>
-  </si>
-  <si>
-    <t>çılgın çiçek</t>
-  </si>
-  <si>
-    <t>cici patates</t>
-  </si>
-  <si>
-    <t>Quickduck</t>
-  </si>
-  <si>
-    <t>FakırKral</t>
-  </si>
-  <si>
-    <t>UçanTekmeCetLi</t>
-  </si>
-  <si>
-    <t>RunAway</t>
-  </si>
-  <si>
-    <t>HomePhobiA</t>
-  </si>
-  <si>
-    <t>cehape</t>
-  </si>
-  <si>
-    <t>MarlonBrando</t>
-  </si>
-  <si>
-    <t>NaylonBranda</t>
-  </si>
-  <si>
-    <t>SweetHomeBursa</t>
-  </si>
-  <si>
-    <t>Tarhanatula</t>
   </si>
 </sst>
 </file>
@@ -1302,18 +1266,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C151"/>
+  <dimension ref="A1:D139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="A152" sqref="A152"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" customWidth="1"/>
+    <col min="1" max="1" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1321,10 +1283,15 @@
         <v>137</v>
       </c>
       <c r="C1">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <f ca="1">RANDBETWEEN(50,300)*30</f>
+        <v>8280</v>
+      </c>
+      <c r="D1">
+        <f ca="1">IF(C1&lt;3500,0,IF(C1&lt;7000,1,2))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1332,10 +1299,15 @@
         <v>136</v>
       </c>
       <c r="C2">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ref="C2:C65" ca="1" si="0">RANDBETWEEN(50,300)*30</f>
+        <v>8880</v>
+      </c>
+      <c r="D2">
+        <f t="shared" ref="D2:D65" ca="1" si="1">IF(C2&lt;3500,0,IF(C2&lt;7000,1,2))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1343,10 +1315,15 @@
         <v>136</v>
       </c>
       <c r="C3">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>2820</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1354,10 +1331,15 @@
         <v>137</v>
       </c>
       <c r="C4">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>5340</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1365,10 +1347,15 @@
         <v>136</v>
       </c>
       <c r="C5">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>7980</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1376,10 +1363,15 @@
         <v>137</v>
       </c>
       <c r="C6">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>7500</v>
+      </c>
+      <c r="D6">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1387,10 +1379,15 @@
         <v>137</v>
       </c>
       <c r="C7">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>1770</v>
+      </c>
+      <c r="D7">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1398,10 +1395,15 @@
         <v>137</v>
       </c>
       <c r="C8">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>6360</v>
+      </c>
+      <c r="D8">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1409,10 +1411,15 @@
         <v>137</v>
       </c>
       <c r="C9">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>6510</v>
+      </c>
+      <c r="D9">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1420,10 +1427,15 @@
         <v>136</v>
       </c>
       <c r="C10">
-        <v>8000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>2460</v>
+      </c>
+      <c r="D10">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1431,10 +1443,15 @@
         <v>137</v>
       </c>
       <c r="C11">
-        <v>8000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>7650</v>
+      </c>
+      <c r="D11">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1442,10 +1459,15 @@
         <v>137</v>
       </c>
       <c r="C12">
-        <v>8000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>6180</v>
+      </c>
+      <c r="D12">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1453,10 +1475,15 @@
         <v>137</v>
       </c>
       <c r="C13">
-        <v>8000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>4170</v>
+      </c>
+      <c r="D13">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1464,10 +1491,15 @@
         <v>136</v>
       </c>
       <c r="C14">
-        <v>8000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>5310</v>
+      </c>
+      <c r="D14">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1475,10 +1507,15 @@
         <v>137</v>
       </c>
       <c r="C15">
-        <v>8000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>8100</v>
+      </c>
+      <c r="D15">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1486,10 +1523,15 @@
         <v>137</v>
       </c>
       <c r="C16">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>3000</v>
+      </c>
+      <c r="D16">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1497,10 +1539,15 @@
         <v>137</v>
       </c>
       <c r="C17">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>4200</v>
+      </c>
+      <c r="D17">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -1508,10 +1555,15 @@
         <v>137</v>
       </c>
       <c r="C18">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>8370</v>
+      </c>
+      <c r="D18">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1519,10 +1571,15 @@
         <v>137</v>
       </c>
       <c r="C19">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>8190</v>
+      </c>
+      <c r="D19">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1530,10 +1587,15 @@
         <v>137</v>
       </c>
       <c r="C20">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>7500</v>
+      </c>
+      <c r="D20">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1541,10 +1603,15 @@
         <v>137</v>
       </c>
       <c r="C21">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>8640</v>
+      </c>
+      <c r="D21">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1552,10 +1619,15 @@
         <v>137</v>
       </c>
       <c r="C22">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>3780</v>
+      </c>
+      <c r="D22">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1563,10 +1635,15 @@
         <v>137</v>
       </c>
       <c r="C23">
-        <v>13000</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>7950</v>
+      </c>
+      <c r="D23">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1574,10 +1651,15 @@
         <v>137</v>
       </c>
       <c r="C24">
-        <v>13000</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>5550</v>
+      </c>
+      <c r="D24">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1585,10 +1667,15 @@
         <v>137</v>
       </c>
       <c r="C25">
-        <v>13000</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>7860</v>
+      </c>
+      <c r="D25">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1596,10 +1683,15 @@
         <v>136</v>
       </c>
       <c r="C26">
-        <v>13000</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>6480</v>
+      </c>
+      <c r="D26">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1607,10 +1699,15 @@
         <v>137</v>
       </c>
       <c r="C27">
-        <v>13000</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>6360</v>
+      </c>
+      <c r="D27">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1618,10 +1715,15 @@
         <v>137</v>
       </c>
       <c r="C28">
-        <v>13000</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>2010</v>
+      </c>
+      <c r="D28">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -1629,10 +1731,15 @@
         <v>137</v>
       </c>
       <c r="C29">
-        <v>15000</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>6300</v>
+      </c>
+      <c r="D29">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1640,10 +1747,15 @@
         <v>137</v>
       </c>
       <c r="C30">
-        <v>15000</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>6810</v>
+      </c>
+      <c r="D30">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -1651,10 +1763,15 @@
         <v>137</v>
       </c>
       <c r="C31">
-        <v>15000</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>6180</v>
+      </c>
+      <c r="D31">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -1662,10 +1779,15 @@
         <v>137</v>
       </c>
       <c r="C32">
-        <v>15000</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>3090</v>
+      </c>
+      <c r="D32">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -1673,10 +1795,15 @@
         <v>137</v>
       </c>
       <c r="C33">
-        <v>15000</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>3270</v>
+      </c>
+      <c r="D33">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -1684,10 +1811,15 @@
         <v>137</v>
       </c>
       <c r="C34">
-        <v>15000</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>2610</v>
+      </c>
+      <c r="D34">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -1695,10 +1827,15 @@
         <v>137</v>
       </c>
       <c r="C35">
-        <v>18000</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>6930</v>
+      </c>
+      <c r="D35">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -1706,10 +1843,15 @@
         <v>137</v>
       </c>
       <c r="C36">
-        <v>18000</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>1500</v>
+      </c>
+      <c r="D36">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -1717,10 +1859,15 @@
         <v>137</v>
       </c>
       <c r="C37">
-        <v>18000</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>7290</v>
+      </c>
+      <c r="D37">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -1728,10 +1875,15 @@
         <v>137</v>
       </c>
       <c r="C38">
-        <v>18000</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>2520</v>
+      </c>
+      <c r="D38">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -1739,10 +1891,15 @@
         <v>137</v>
       </c>
       <c r="C39">
-        <v>18000</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>1920</v>
+      </c>
+      <c r="D39">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -1750,10 +1907,15 @@
         <v>137</v>
       </c>
       <c r="C40">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>4260</v>
+      </c>
+      <c r="D40">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -1761,10 +1923,15 @@
         <v>137</v>
       </c>
       <c r="C41">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>3510</v>
+      </c>
+      <c r="D41">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -1772,10 +1939,15 @@
         <v>137</v>
       </c>
       <c r="C42">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>3420</v>
+      </c>
+      <c r="D42">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -1783,10 +1955,15 @@
         <v>136</v>
       </c>
       <c r="C43">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>6480</v>
+      </c>
+      <c r="D43">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -1794,10 +1971,15 @@
         <v>137</v>
       </c>
       <c r="C44">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>6510</v>
+      </c>
+      <c r="D44">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -1805,10 +1987,15 @@
         <v>137</v>
       </c>
       <c r="C45">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>7680</v>
+      </c>
+      <c r="D45">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -1816,10 +2003,15 @@
         <v>137</v>
       </c>
       <c r="C46">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>5310</v>
+      </c>
+      <c r="D46">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -1827,10 +2019,15 @@
         <v>137</v>
       </c>
       <c r="C47">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>7860</v>
+      </c>
+      <c r="D47">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -1838,10 +2035,15 @@
         <v>137</v>
       </c>
       <c r="C48">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>2280</v>
+      </c>
+      <c r="D48">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -1849,10 +2051,15 @@
         <v>136</v>
       </c>
       <c r="C49">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>8640</v>
+      </c>
+      <c r="D49">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -1860,10 +2067,15 @@
         <v>137</v>
       </c>
       <c r="C50">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>7800</v>
+      </c>
+      <c r="D50">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -1871,10 +2083,15 @@
         <v>137</v>
       </c>
       <c r="C51">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>2220</v>
+      </c>
+      <c r="D51">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -1882,10 +2099,15 @@
         <v>136</v>
       </c>
       <c r="C52">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>2100</v>
+      </c>
+      <c r="D52">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -1893,10 +2115,15 @@
         <v>136</v>
       </c>
       <c r="C53">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>1620</v>
+      </c>
+      <c r="D53">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -1904,10 +2131,15 @@
         <v>136</v>
       </c>
       <c r="C54">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>6300</v>
+      </c>
+      <c r="D54">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>48</v>
       </c>
@@ -1915,10 +2147,15 @@
         <v>136</v>
       </c>
       <c r="C55">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>8550</v>
+      </c>
+      <c r="D55">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>54</v>
       </c>
@@ -1926,10 +2163,15 @@
         <v>137</v>
       </c>
       <c r="C56">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>2610</v>
+      </c>
+      <c r="D56">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>55</v>
       </c>
@@ -1937,10 +2179,15 @@
         <v>136</v>
       </c>
       <c r="C57">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>7140</v>
+      </c>
+      <c r="D57">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>56</v>
       </c>
@@ -1948,10 +2195,15 @@
         <v>137</v>
       </c>
       <c r="C58">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>8670</v>
+      </c>
+      <c r="D58">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>57</v>
       </c>
@@ -1959,10 +2211,15 @@
         <v>136</v>
       </c>
       <c r="C59">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>3210</v>
+      </c>
+      <c r="D59">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>58</v>
       </c>
@@ -1970,10 +2227,15 @@
         <v>137</v>
       </c>
       <c r="C60">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>6120</v>
+      </c>
+      <c r="D60">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>59</v>
       </c>
@@ -1981,10 +2243,15 @@
         <v>136</v>
       </c>
       <c r="C61">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>7290</v>
+      </c>
+      <c r="D61">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>60</v>
       </c>
@@ -1992,10 +2259,15 @@
         <v>136</v>
       </c>
       <c r="C62">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>6870</v>
+      </c>
+      <c r="D62">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>61</v>
       </c>
@@ -2003,10 +2275,15 @@
         <v>137</v>
       </c>
       <c r="C63">
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>5310</v>
+      </c>
+      <c r="D63">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>62</v>
       </c>
@@ -2014,10 +2291,15 @@
         <v>136</v>
       </c>
       <c r="C64">
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>3390</v>
+      </c>
+      <c r="D64">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>63</v>
       </c>
@@ -2025,10 +2307,15 @@
         <v>136</v>
       </c>
       <c r="C65">
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>5100</v>
+      </c>
+      <c r="D65">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>64</v>
       </c>
@@ -2036,10 +2323,15 @@
         <v>137</v>
       </c>
       <c r="C66">
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ref="C66:C129" ca="1" si="2">RANDBETWEEN(50,300)*30</f>
+        <v>8340</v>
+      </c>
+      <c r="D66">
+        <f t="shared" ref="D66:D129" ca="1" si="3">IF(C66&lt;3500,0,IF(C66&lt;7000,1,2))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>65</v>
       </c>
@@ -2047,10 +2339,15 @@
         <v>136</v>
       </c>
       <c r="C67">
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>5490</v>
+      </c>
+      <c r="D67">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>66</v>
       </c>
@@ -2058,10 +2355,15 @@
         <v>136</v>
       </c>
       <c r="C68">
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>5280</v>
+      </c>
+      <c r="D68">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>67</v>
       </c>
@@ -2069,10 +2371,15 @@
         <v>137</v>
       </c>
       <c r="C69">
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>5580</v>
+      </c>
+      <c r="D69">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>68</v>
       </c>
@@ -2080,10 +2387,15 @@
         <v>137</v>
       </c>
       <c r="C70">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>3510</v>
+      </c>
+      <c r="D70">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>69</v>
       </c>
@@ -2091,10 +2403,15 @@
         <v>136</v>
       </c>
       <c r="C71">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>5220</v>
+      </c>
+      <c r="D71">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>70</v>
       </c>
@@ -2102,10 +2419,15 @@
         <v>137</v>
       </c>
       <c r="C72">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>6600</v>
+      </c>
+      <c r="D72">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>71</v>
       </c>
@@ -2113,10 +2435,15 @@
         <v>137</v>
       </c>
       <c r="C73">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>5250</v>
+      </c>
+      <c r="D73">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>72</v>
       </c>
@@ -2124,10 +2451,15 @@
         <v>137</v>
       </c>
       <c r="C74">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>6360</v>
+      </c>
+      <c r="D74">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>73</v>
       </c>
@@ -2135,10 +2467,15 @@
         <v>137</v>
       </c>
       <c r="C75">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>6960</v>
+      </c>
+      <c r="D75">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>74</v>
       </c>
@@ -2146,10 +2483,15 @@
         <v>136</v>
       </c>
       <c r="C76">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>5820</v>
+      </c>
+      <c r="D76">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>75</v>
       </c>
@@ -2157,10 +2499,15 @@
         <v>137</v>
       </c>
       <c r="C77">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>3150</v>
+      </c>
+      <c r="D77">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>76</v>
       </c>
@@ -2168,10 +2515,15 @@
         <v>136</v>
       </c>
       <c r="C78">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>7500</v>
+      </c>
+      <c r="D78">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>77</v>
       </c>
@@ -2179,10 +2531,15 @@
         <v>137</v>
       </c>
       <c r="C79">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>4170</v>
+      </c>
+      <c r="D79">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>78</v>
       </c>
@@ -2190,10 +2547,15 @@
         <v>137</v>
       </c>
       <c r="C80">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>4170</v>
+      </c>
+      <c r="D80">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>79</v>
       </c>
@@ -2201,10 +2563,15 @@
         <v>137</v>
       </c>
       <c r="C81">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>7470</v>
+      </c>
+      <c r="D81">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>80</v>
       </c>
@@ -2212,10 +2579,15 @@
         <v>137</v>
       </c>
       <c r="C82">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>4710</v>
+      </c>
+      <c r="D82">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>81</v>
       </c>
@@ -2223,10 +2595,15 @@
         <v>136</v>
       </c>
       <c r="C83">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>3240</v>
+      </c>
+      <c r="D83">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>82</v>
       </c>
@@ -2234,10 +2611,15 @@
         <v>136</v>
       </c>
       <c r="C84">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>8760</v>
+      </c>
+      <c r="D84">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>83</v>
       </c>
@@ -2245,10 +2627,15 @@
         <v>136</v>
       </c>
       <c r="C85">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>2250</v>
+      </c>
+      <c r="D85">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>84</v>
       </c>
@@ -2256,10 +2643,15 @@
         <v>136</v>
       </c>
       <c r="C86">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>6240</v>
+      </c>
+      <c r="D86">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>85</v>
       </c>
@@ -2267,10 +2659,15 @@
         <v>136</v>
       </c>
       <c r="C87">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>3270</v>
+      </c>
+      <c r="D87">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>86</v>
       </c>
@@ -2278,10 +2675,15 @@
         <v>136</v>
       </c>
       <c r="C88">
-        <v>45000</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>3240</v>
+      </c>
+      <c r="D88">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>87</v>
       </c>
@@ -2289,10 +2691,15 @@
         <v>136</v>
       </c>
       <c r="C89">
-        <v>45000</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>8190</v>
+      </c>
+      <c r="D89">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>88</v>
       </c>
@@ -2300,10 +2707,15 @@
         <v>136</v>
       </c>
       <c r="C90">
-        <v>45000</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>2580</v>
+      </c>
+      <c r="D90">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>89</v>
       </c>
@@ -2311,10 +2723,15 @@
         <v>137</v>
       </c>
       <c r="C91">
-        <v>45000</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>8940</v>
+      </c>
+      <c r="D91">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>90</v>
       </c>
@@ -2322,10 +2739,15 @@
         <v>136</v>
       </c>
       <c r="C92">
-        <v>45000</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>5190</v>
+      </c>
+      <c r="D92">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>91</v>
       </c>
@@ -2333,10 +2755,15 @@
         <v>136</v>
       </c>
       <c r="C93">
-        <v>45000</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>3450</v>
+      </c>
+      <c r="D93">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>92</v>
       </c>
@@ -2344,10 +2771,15 @@
         <v>136</v>
       </c>
       <c r="C94">
-        <v>45000</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>8730</v>
+      </c>
+      <c r="D94">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>93</v>
       </c>
@@ -2355,10 +2787,15 @@
         <v>137</v>
       </c>
       <c r="C95">
-        <v>45000</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>1590</v>
+      </c>
+      <c r="D95">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>94</v>
       </c>
@@ -2366,10 +2803,15 @@
         <v>136</v>
       </c>
       <c r="C96">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>2880</v>
+      </c>
+      <c r="D96">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>95</v>
       </c>
@@ -2377,10 +2819,15 @@
         <v>137</v>
       </c>
       <c r="C97">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>4800</v>
+      </c>
+      <c r="D97">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>96</v>
       </c>
@@ -2388,10 +2835,15 @@
         <v>137</v>
       </c>
       <c r="C98">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>7770</v>
+      </c>
+      <c r="D98">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>97</v>
       </c>
@@ -2399,10 +2851,15 @@
         <v>137</v>
       </c>
       <c r="C99">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>4500</v>
+      </c>
+      <c r="D99">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>98</v>
       </c>
@@ -2410,10 +2867,15 @@
         <v>137</v>
       </c>
       <c r="C100">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>6210</v>
+      </c>
+      <c r="D100">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>99</v>
       </c>
@@ -2421,10 +2883,15 @@
         <v>136</v>
       </c>
       <c r="C101">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>7320</v>
+      </c>
+      <c r="D101">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>100</v>
       </c>
@@ -2432,10 +2899,15 @@
         <v>137</v>
       </c>
       <c r="C102">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>3600</v>
+      </c>
+      <c r="D102">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>101</v>
       </c>
@@ -2443,10 +2915,15 @@
         <v>136</v>
       </c>
       <c r="C103">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>2910</v>
+      </c>
+      <c r="D103">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>102</v>
       </c>
@@ -2454,10 +2931,15 @@
         <v>137</v>
       </c>
       <c r="C104">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>2160</v>
+      </c>
+      <c r="D104">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>103</v>
       </c>
@@ -2465,10 +2947,15 @@
         <v>137</v>
       </c>
       <c r="C105">
-        <v>8000</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>7320</v>
+      </c>
+      <c r="D105">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>104</v>
       </c>
@@ -2476,10 +2963,15 @@
         <v>137</v>
       </c>
       <c r="C106">
-        <v>8000</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>1710</v>
+      </c>
+      <c r="D106">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>105</v>
       </c>
@@ -2487,10 +2979,15 @@
         <v>136</v>
       </c>
       <c r="C107">
-        <v>8000</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>6060</v>
+      </c>
+      <c r="D107">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>106</v>
       </c>
@@ -2498,10 +2995,15 @@
         <v>137</v>
       </c>
       <c r="C108">
-        <v>8000</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>5010</v>
+      </c>
+      <c r="D108">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>107</v>
       </c>
@@ -2509,10 +3011,15 @@
         <v>136</v>
       </c>
       <c r="C109">
-        <v>8000</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>7260</v>
+      </c>
+      <c r="D109">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>108</v>
       </c>
@@ -2520,10 +3027,15 @@
         <v>137</v>
       </c>
       <c r="C110">
-        <v>8000</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>5190</v>
+      </c>
+      <c r="D110">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>109</v>
       </c>
@@ -2531,10 +3043,15 @@
         <v>137</v>
       </c>
       <c r="C111">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>1620</v>
+      </c>
+      <c r="D111">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>110</v>
       </c>
@@ -2542,10 +3059,15 @@
         <v>137</v>
       </c>
       <c r="C112">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>5670</v>
+      </c>
+      <c r="D112">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>111</v>
       </c>
@@ -2553,10 +3075,15 @@
         <v>137</v>
       </c>
       <c r="C113">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>5730</v>
+      </c>
+      <c r="D113">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>112</v>
       </c>
@@ -2564,10 +3091,15 @@
         <v>137</v>
       </c>
       <c r="C114">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>3810</v>
+      </c>
+      <c r="D114">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>113</v>
       </c>
@@ -2575,10 +3107,15 @@
         <v>137</v>
       </c>
       <c r="C115">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>8970</v>
+      </c>
+      <c r="D115">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>114</v>
       </c>
@@ -2586,10 +3123,15 @@
         <v>137</v>
       </c>
       <c r="C116">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>3300</v>
+      </c>
+      <c r="D116">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>115</v>
       </c>
@@ -2597,10 +3139,15 @@
         <v>137</v>
       </c>
       <c r="C117">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>3570</v>
+      </c>
+      <c r="D117">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>116</v>
       </c>
@@ -2608,10 +3155,15 @@
         <v>137</v>
       </c>
       <c r="C118">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>1500</v>
+      </c>
+      <c r="D118">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>117</v>
       </c>
@@ -2619,10 +3171,15 @@
         <v>137</v>
       </c>
       <c r="C119">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>7650</v>
+      </c>
+      <c r="D119">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>118</v>
       </c>
@@ -2630,10 +3187,15 @@
         <v>137</v>
       </c>
       <c r="C120">
-        <v>8000</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>3330</v>
+      </c>
+      <c r="D120">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>119</v>
       </c>
@@ -2641,10 +3203,15 @@
         <v>137</v>
       </c>
       <c r="C121">
-        <v>8000</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>5070</v>
+      </c>
+      <c r="D121">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>120</v>
       </c>
@@ -2652,10 +3219,15 @@
         <v>136</v>
       </c>
       <c r="C122">
-        <v>8000</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>7080</v>
+      </c>
+      <c r="D122">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>121</v>
       </c>
@@ -2663,10 +3235,15 @@
         <v>137</v>
       </c>
       <c r="C123">
-        <v>8000</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>4290</v>
+      </c>
+      <c r="D123">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>122</v>
       </c>
@@ -2674,10 +3251,15 @@
         <v>137</v>
       </c>
       <c r="C124">
-        <v>8000</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>4950</v>
+      </c>
+      <c r="D124">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>123</v>
       </c>
@@ -2685,10 +3267,15 @@
         <v>137</v>
       </c>
       <c r="C125">
-        <v>90000</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>7110</v>
+      </c>
+      <c r="D125">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>124</v>
       </c>
@@ -2696,10 +3283,15 @@
         <v>137</v>
       </c>
       <c r="C126">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>6480</v>
+      </c>
+      <c r="D126">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>125</v>
       </c>
@@ -2707,10 +3299,15 @@
         <v>137</v>
       </c>
       <c r="C127">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>3630</v>
+      </c>
+      <c r="D127">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>126</v>
       </c>
@@ -2718,10 +3315,15 @@
         <v>136</v>
       </c>
       <c r="C128">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>3360</v>
+      </c>
+      <c r="D128">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>127</v>
       </c>
@@ -2729,10 +3331,15 @@
         <v>137</v>
       </c>
       <c r="C129">
-        <v>85000</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>6840</v>
+      </c>
+      <c r="D129">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>128</v>
       </c>
@@ -2740,10 +3347,15 @@
         <v>137</v>
       </c>
       <c r="C130">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ref="C130:C139" ca="1" si="4">RANDBETWEEN(50,300)*30</f>
+        <v>3240</v>
+      </c>
+      <c r="D130">
+        <f t="shared" ref="D130:D139" ca="1" si="5">IF(C130&lt;3500,0,IF(C130&lt;7000,1,2))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>129</v>
       </c>
@@ -2751,10 +3363,15 @@
         <v>136</v>
       </c>
       <c r="C131">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="4"/>
+        <v>4110</v>
+      </c>
+      <c r="D131">
+        <f t="shared" ca="1" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>130</v>
       </c>
@@ -2762,10 +3379,15 @@
         <v>137</v>
       </c>
       <c r="C132">
-        <v>120000</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="4"/>
+        <v>5760</v>
+      </c>
+      <c r="D132">
+        <f t="shared" ca="1" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>131</v>
       </c>
@@ -2773,10 +3395,15 @@
         <v>137</v>
       </c>
       <c r="C133">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="4"/>
+        <v>1980</v>
+      </c>
+      <c r="D133">
+        <f t="shared" ca="1" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>132</v>
       </c>
@@ -2784,10 +3411,15 @@
         <v>137</v>
       </c>
       <c r="C134">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="4"/>
+        <v>2430</v>
+      </c>
+      <c r="D134">
+        <f t="shared" ca="1" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>133</v>
       </c>
@@ -2795,10 +3427,15 @@
         <v>136</v>
       </c>
       <c r="C135">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="4"/>
+        <v>5010</v>
+      </c>
+      <c r="D135">
+        <f t="shared" ca="1" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>134</v>
       </c>
@@ -2806,10 +3443,15 @@
         <v>137</v>
       </c>
       <c r="C136">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="4"/>
+        <v>6720</v>
+      </c>
+      <c r="D136">
+        <f t="shared" ca="1" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>135</v>
       </c>
@@ -2817,10 +3459,15 @@
         <v>137</v>
       </c>
       <c r="C137">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="4"/>
+        <v>5100</v>
+      </c>
+      <c r="D137">
+        <f t="shared" ca="1" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>138</v>
       </c>
@@ -2828,10 +3475,15 @@
         <v>137</v>
       </c>
       <c r="C138">
-        <v>60000</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="4"/>
+        <v>5040</v>
+      </c>
+      <c r="D138">
+        <f t="shared" ca="1" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>139</v>
       </c>
@@ -2839,139 +3491,12 @@
         <v>140</v>
       </c>
       <c r="C139">
-        <v>33000</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
-        <v>141</v>
-      </c>
-      <c r="B140" t="s">
-        <v>140</v>
-      </c>
-      <c r="C140">
-        <v>5200</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
-        <v>142</v>
-      </c>
-      <c r="B141" t="s">
-        <v>140</v>
-      </c>
-      <c r="C141">
-        <v>6000</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
-        <v>143</v>
-      </c>
-      <c r="B142" t="s">
-        <v>137</v>
-      </c>
-      <c r="C142">
-        <v>7500</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
-        <v>151</v>
-      </c>
-      <c r="B143" t="s">
-        <v>140</v>
-      </c>
-      <c r="C143">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
-        <v>146</v>
-      </c>
-      <c r="B144" t="s">
-        <v>140</v>
-      </c>
-      <c r="C144">
-        <v>15000</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
-        <v>147</v>
-      </c>
-      <c r="B145" t="s">
-        <v>140</v>
-      </c>
-      <c r="C145">
-        <v>18000</v>
-      </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
-        <v>144</v>
-      </c>
-      <c r="B146" t="s">
-        <v>137</v>
-      </c>
-      <c r="C146">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
-        <v>145</v>
-      </c>
-      <c r="B147" t="s">
-        <v>137</v>
-      </c>
-      <c r="C147">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
-        <v>148</v>
-      </c>
-      <c r="B148" t="s">
-        <v>137</v>
-      </c>
-      <c r="C148">
-        <v>8000</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
-        <v>149</v>
-      </c>
-      <c r="B149" t="s">
-        <v>137</v>
-      </c>
-      <c r="C149">
-        <v>15000</v>
-      </c>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A150" t="s">
-        <v>150</v>
-      </c>
-      <c r="B150" t="s">
-        <v>137</v>
-      </c>
-      <c r="C150">
-        <v>22000</v>
-      </c>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
-        <v>152</v>
-      </c>
-      <c r="B151" t="s">
-        <v>140</v>
-      </c>
-      <c r="C151">
-        <v>58000</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>3990</v>
+      </c>
+      <c r="D139">
+        <f t="shared" ca="1" si="5"/>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>